<commit_message>
Account AutoIncrement 옵션 누락
</commit_message>
<xml_diff>
--- a/Data/Excel/Model/Auth/Account.xlsx
+++ b/Data/Excel/Model/Auth/Account.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Model\User\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Model\Auth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49611ABD-CBF9-4BCF-AC98-B07FF86162EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7279A0-8C80-4F03-BF48-D88B2E974CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="795" yWindow="825" windowWidth="12750" windowHeight="11295" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
@@ -62,10 +62,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>pk</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Id</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -91,6 +87,10 @@
   </si>
   <si>
     <t>VARCHAR(50)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pk, autogenerated</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1028,7 +1028,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1060,7 +1060,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1069,12 +1069,12 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1085,20 +1085,20 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>

</xml_diff>